<commit_message>
Update TP biochimie14/11/2020 19h07 A1: ajout de photo, correction de orthographe, tableau excel (a refaire) A2: ajout image et vérification ortho A4: reformulation de la méthode et ajout image Derycke Emeline
</commit_message>
<xml_diff>
--- a/Excel/brad1.xlsx
+++ b/Excel/brad1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11101"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\VirtualBox VMs\SciViews Box 2020\shared\projects\TP-Bioch-BAB2-Q1\Dataframes Excel (.xlsx)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emelinederycke/VirtualBox VMs/SciViews Box 2020/shared/projects/TP-Bioch-BAB2-Q1/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F552CABB-8487-4C2A-996F-3EB782C2646C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6449E86B-3CC7-5A4D-BF94-948D02D0682C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="3570" windowWidth="21600" windowHeight="11385" xr2:uid="{2D845E35-5265-4FEA-AA1A-06CD67E70E09}"/>
+    <workbookView xWindow="5080" yWindow="3580" windowWidth="21600" windowHeight="11380" xr2:uid="{2D845E35-5265-4FEA-AA1A-06CD67E70E09}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>6’’</t>
   </si>
   <si>
-    <t>Albumine à 1 mg/ml (µl)</t>
-  </si>
-  <si>
     <t>Eau distillée (µl)</t>
   </si>
   <si>
@@ -95,17 +92,20 @@
     <t>D.O. à 595 nm - blanc</t>
   </si>
   <si>
-    <t>0.005 NEG</t>
-  </si>
-  <si>
-    <t>0.013 NEG</t>
+    <t>Albumine à 1,58 mg/ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le groupe 3 a changé </t>
+  </si>
+  <si>
+    <t>0,0158mg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +132,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Corps)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -201,11 +214,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -243,8 +270,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,39 +590,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE2BC35-EA30-4B27-897F-0C7AE16E1ADF}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -603,15 +634,15 @@
         <v>4</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="5">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5">
         <v>0</v>
       </c>
-      <c r="G2" s="5"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -619,15 +650,15 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="5">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
+        <v>-2.1000000000000001E-2</v>
+      </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -635,18 +666,18 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="5">
-        <v>2E-3</v>
-      </c>
-      <c r="G4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5">
+        <v>0.19800000000000001</v>
+      </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
-        <v>10</v>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C5" s="6">
         <v>90</v>
@@ -655,29 +686,31 @@
         <v>4</v>
       </c>
       <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7">
+        <v>0.24299999999999999</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
-        <v>10</v>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G6" s="5"/>
+      <c r="E6" s="5">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
+        <v>0.223</v>
+      </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -687,13 +720,13 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="G7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
+        <v>0.26800000000000002</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -707,13 +740,13 @@
         <v>4</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7">
+        <v>0.26</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -723,13 +756,13 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="G9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
+        <v>0.33400000000000002</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -739,13 +772,13 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="5">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="G10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5">
+        <v>0.38900000000000001</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>4</v>
       </c>
@@ -760,10 +793,12 @@
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7">
+        <v>0.53900000000000003</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -774,10 +809,12 @@
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="G12" s="5">
+        <v>0.36099999999999999</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -788,10 +825,12 @@
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="G13" s="5">
+        <v>0.51900000000000002</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -806,10 +845,12 @@
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="8">
+        <v>0.73299999999999998</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -820,10 +861,12 @@
       <c r="D15" s="4"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9">
+        <v>0.63100000000000001</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -834,10 +877,12 @@
       <c r="D16" s="4"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="9">
+        <v>0.75</v>
+      </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -852,10 +897,12 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7">
+        <v>1.1859999999999999</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -866,10 +913,12 @@
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="G18" s="5">
+        <v>1.1319999999999999</v>
+      </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -880,37 +929,39 @@
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="G19" s="11">
+        <v>1.179</v>
+      </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H29" s="1"/>
     </row>
   </sheetData>

</xml_diff>